<commit_message>
1.17.2_docs: fill competition sign up table
</commit_message>
<xml_diff>
--- a/附件2：2025年上海市大学生计算机应用能力大赛报名汇总表.xlsx
+++ b/附件2：2025年上海市大学生计算机应用能力大赛报名汇总表.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\IDEA Java Code\LinkUp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FDU\Temp\LinkUp\LinkUp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D17393F-D008-4C60-BF4F-6F20A706A838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C786FD73-A6D9-48AA-9658-044C200ABC1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="30940" windowHeight="18700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="75">
   <si>
     <t>作品名称</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -295,12 +295,20 @@
     <t>Link Up</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>330327200405300116</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hcy13245@163.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -23336,11 +23344,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" style="5" customWidth="1"/>
     <col min="2" max="2" width="20.75" style="1" customWidth="1"/>
@@ -23381,7 +23389,7 @@
     <col min="38" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="11" customFormat="1" ht="25" customHeight="1">
+    <row r="1" spans="1:37" s="11" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
@@ -23480,7 +23488,7 @@
       <c r="AJ1" s="9"/>
       <c r="AK1" s="9"/>
     </row>
-    <row r="2" spans="1:37" ht="21" customHeight="1">
+    <row r="2" spans="1:37" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>72</v>
       </c>
@@ -23520,6 +23528,9 @@
       <c r="O2" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="P2" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="Q2" s="1" t="s">
         <v>68</v>
       </c>
@@ -23532,6 +23543,12 @@
       <c r="T2" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="U2" s="1">
+        <v>17706660011</v>
+      </c>
+      <c r="V2" s="13" t="s">
+        <v>74</v>
+      </c>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -23543,9 +23560,10 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="N2" r:id="rId1" xr:uid="{6AF7B727-AB12-4E28-A940-8F4DC4ECA071}"/>
+    <hyperlink ref="V2" r:id="rId2" xr:uid="{A067C481-7920-4F67-A246-614C2DC3E354}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -23557,14 +23575,14 @@
       <selection activeCell="A2" sqref="A2:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.25" customWidth="1"/>
     <col min="2" max="2" width="24.58203125" customWidth="1"/>
     <col min="6" max="6" width="19.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>49</v>
       </c>
@@ -23572,7 +23590,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>38</v>
       </c>
@@ -23580,7 +23598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>48</v>
       </c>
@@ -23588,7 +23606,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>40</v>
       </c>
@@ -23596,7 +23614,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
@@ -23604,7 +23622,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>47</v>
       </c>
@@ -23612,7 +23630,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>41</v>
       </c>
@@ -23620,7 +23638,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>44</v>
       </c>
@@ -23628,7 +23646,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>33</v>
       </c>
@@ -23636,7 +23654,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>43</v>
       </c>
@@ -23644,7 +23662,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>32</v>
       </c>
@@ -23652,7 +23670,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>42</v>
       </c>
@@ -23660,7 +23678,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>46</v>
       </c>
@@ -23668,7 +23686,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>45</v>
       </c>
@@ -23676,7 +23694,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>34</v>
       </c>
@@ -23684,7 +23702,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>29</v>
       </c>
@@ -23692,7 +23710,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>31</v>
       </c>
@@ -23700,7 +23718,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>39</v>
       </c>
@@ -23708,7 +23726,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>35</v>
       </c>
@@ -23716,7 +23734,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>36</v>
       </c>
@@ -23724,7 +23742,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>37</v>
       </c>
@@ -23732,7 +23750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>50</v>
       </c>
@@ -23740,7 +23758,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>51</v>
       </c>
@@ -23762,13 +23780,13 @@
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="22.58203125" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5">
+    <row r="2" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C2" s="12" t="s">
         <v>53</v>
       </c>
@@ -23776,7 +23794,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="3:5">
+    <row r="3" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C3" s="12" t="s">
         <v>48</v>
       </c>
@@ -23784,7 +23802,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="3:5">
+    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C4" s="12" t="s">
         <v>40</v>
       </c>
@@ -23792,7 +23810,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="3:5">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C5" s="12" t="s">
         <v>30</v>
       </c>
@@ -23800,13 +23818,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="3:5">
+    <row r="6" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C6" s="12" t="s">
         <v>54</v>
       </c>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="3:5">
+    <row r="7" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C7" s="12" t="s">
         <v>47</v>
       </c>
@@ -23814,7 +23832,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="3:5">
+    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C8" s="12" t="s">
         <v>41</v>
       </c>
@@ -23822,13 +23840,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="3:5">
+    <row r="9" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C9" s="12"/>
       <c r="E9" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="3:5">
+    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C10" s="12" t="s">
         <v>55</v>
       </c>
@@ -23836,13 +23854,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="3:5">
+    <row r="11" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C11" s="12" t="s">
         <v>56</v>
       </c>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="3:5">
+    <row r="12" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C12" s="12" t="s">
         <v>43</v>
       </c>
@@ -23850,7 +23868,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="3:5">
+    <row r="13" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C13" s="12" t="s">
         <v>32</v>
       </c>
@@ -23858,19 +23876,19 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="3:5">
+    <row r="14" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C14" s="12" t="s">
         <v>57</v>
       </c>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="3:5">
+    <row r="15" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C15" s="12" t="s">
         <v>58</v>
       </c>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="3:5">
+    <row r="16" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C16" s="12" t="s">
         <v>42</v>
       </c>
@@ -23878,13 +23896,13 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="3:5">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C17" s="12" t="s">
         <v>59</v>
       </c>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="3:5">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C18" s="12" t="s">
         <v>46</v>
       </c>
@@ -23892,7 +23910,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="3:5">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C19" s="12" t="s">
         <v>45</v>
       </c>
@@ -23900,13 +23918,13 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="3:5">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C20" s="12"/>
       <c r="E20" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="3:5">
+    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C21" s="12" t="s">
         <v>29</v>
       </c>
@@ -23914,7 +23932,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="3:5">
+    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C22" s="12" t="s">
         <v>31</v>
       </c>
@@ -23922,7 +23940,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="3:5">
+    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C23" s="12" t="s">
         <v>39</v>
       </c>
@@ -23930,7 +23948,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="3:5">
+    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C24" s="12" t="s">
         <v>35</v>
       </c>
@@ -23938,13 +23956,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="3:5">
+    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C25" s="12" t="s">
         <v>60</v>
       </c>
       <c r="E25" s="4"/>
     </row>
-    <row r="26" spans="3:5">
+    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C26" s="12" t="s">
         <v>36</v>
       </c>
@@ -23952,13 +23970,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="3:5">
+    <row r="27" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C27" s="12" t="s">
         <v>61</v>
       </c>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="3:5">
+    <row r="28" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C28" s="12" t="s">
         <v>37</v>
       </c>
@@ -23966,7 +23984,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="3:5">
+    <row r="29" spans="3:5" x14ac:dyDescent="0.3">
       <c r="E29" s="4" t="s">
         <v>50</v>
       </c>
@@ -23988,109 +24006,109 @@
       <selection activeCell="E2" sqref="E2:E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="5:5">
+    <row r="2" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E2" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="5:5">
+    <row r="3" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E3" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="5:5">
+    <row r="4" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E4" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="5:5">
+    <row r="5" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E5" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="5:5">
+    <row r="6" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E6" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="5:5">
+    <row r="7" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E7" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="5:5">
+    <row r="8" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E8" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="5:5">
+    <row r="9" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E9" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="5:5">
+    <row r="10" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E10" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="5:5">
+    <row r="11" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E11" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="5:5">
+    <row r="12" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E12" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="5:5">
+    <row r="13" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E13" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="5:5">
+    <row r="14" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E14" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="5:5">
+    <row r="15" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E15" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="5:5">
+    <row r="16" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E16" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="5:5">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="5:5">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E18" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="5:5">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E19" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="5:5">
+    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E20" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="5:5">
+    <row r="21" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E21" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="5:5">
+    <row r="22" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E22" s="4" t="s">
         <v>50</v>
       </c>

</xml_diff>